<commit_message>
fix test and checklist
fix test and checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/emanuele_bianchi_dedalus_eu/Documents/Documenti/Production/FSE2.0/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/emanuele_bianchi_dedalus_eu/Documents/Documenti/Production/FSE2.0/S1#111DEDALUS0000_SecondPR/DEDALUS/WHOSPITAL/28.6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="11_E5844F8BE441DE9AE0E2741B1C08B253CC0EFC9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45F9CCBA-8589-4C24-8854-0D749AA478F2}"/>
+  <xr:revisionPtr revIDLastSave="287" documentId="11_E5844F8BE441DE9AE0E2741B1C08B253CC0EFC9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EAA9EF-D5BB-4E9B-8E8E-DCF654B451EE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="143">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -557,42 +557,6 @@
 Non è quindi possibile valorizzare l'entry con dati strutturati</t>
   </si>
   <si>
-    <t>cc9c0cc072541ac9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.9d5cbf28d70547bd24a0bb7f7a2b9b56a737695ac1d6218b11a5987dda1cd165.a7a2f92509^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-17T12:03:12Z</t>
-  </si>
-  <si>
-    <t>2023-02-17T15:35:19Z</t>
-  </si>
-  <si>
-    <t>03886b993b1b4691</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.55525654a514baf7a398afa7d67fa1706731067b3623f6d0df91a6df24d17615.c2fac55069^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-17T15:54:18Z</t>
-  </si>
-  <si>
-    <t>309768cf04d36d6b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.d335952594ed68ed927e9b7c45159377a49cb9c096594839260991fd8006ab7d.042c6f6417^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-17T16:03:07Z</t>
-  </si>
-  <si>
-    <t>f630f028b341fce4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.83e4b49a702cf8de8303e5df79e57a513719b884b1d72b0adef6de72e894a9c8.109974f820^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>La sezione Anamnesi riporta un riassunto testuale dell'anamnesi registrata in cartella; non è pertanto presente in LDO il dato strutturato
 La sezione Terapia_Farmacologica_Ingresso riporta un riassunto testuale delle terapia all'ingresso; non è pertanto presente in LDO il dato strutturato
 La sezione Terapia_farmacologica_dimissione riporta un riassunto testuale della terapia alla dimissione; non è pertanto presente in LDO il dato strutturato</t>
@@ -701,6 +665,42 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.30922.4.4.7357ebe77d8b19fad8fcfb510ed29df4b89c94412e7e5d6ac5f660e59b2d2407.6064d3e95e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-15T10:16:43Z</t>
+  </si>
+  <si>
+    <t>32024f65c5b09cd8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.57eb4e049b0d33aeb034be70b5e9175d73e1e6d8b94dd9ef64cc27e90b4f5901.a01731730d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-15T10:23:25Z</t>
+  </si>
+  <si>
+    <t>c3cafdab2dda3a5e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.548fb5c0eea3e1f235feda2bf0962e5d9eb83833ec1d85e8b361515ebdd30c65.d46a21d443^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-15T10:31:03Z</t>
+  </si>
+  <si>
+    <t>dd15863c397c18d7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.cb3d023c0bca1ccc0ef42aa132e292243dac5f08f847ac9da0ea1316ad119b82.b621c5e9ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-15T10:36:49Z</t>
+  </si>
+  <si>
+    <t>b0825debc2f2aa97</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.8e09bb6d0d285f084c7e1e68c7806cc39296063545601bf6387cf5c84504c8aa.521e3ef2fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1264,6 +1264,15 @@
     <xf numFmtId="21" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1285,15 +1294,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2663,11 +2663,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O873"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2698,12 +2698,12 @@
       <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="33" hidden="1" customHeight="1">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="52"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -2716,14 +2716,14 @@
       <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" hidden="1" customHeight="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="52"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -2736,12 +2736,12 @@
       <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" ht="14.25" hidden="1" customHeight="1">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="57" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -2755,12 +2755,12 @@
       <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" hidden="1" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="52"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -2773,8 +2773,8 @@
       <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:15" ht="14.25" hidden="1" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="12"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2827,7 +2827,7 @@
       <c r="D9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="47" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="15" t="s">
@@ -2878,16 +2878,16 @@
         <v>32</v>
       </c>
       <c r="F10" s="20">
-        <v>44974</v>
+        <v>45000</v>
       </c>
       <c r="G10" s="45" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
@@ -2900,7 +2900,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="24"/>
     </row>
-    <row r="11" spans="1:15" ht="150.75" thickBot="1">
+    <row r="11" spans="1:15" ht="210.75" thickBot="1">
       <c r="A11" s="17">
         <v>7</v>
       </c>
@@ -2917,29 +2917,27 @@
         <v>34</v>
       </c>
       <c r="F11" s="20">
-        <v>44974</v>
+        <v>45000</v>
       </c>
       <c r="G11" s="45" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="M11" s="22"/>
+        <v>91</v>
+      </c>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="N11" s="23"/>
-      <c r="O11" s="58" t="s">
-        <v>107</v>
-      </c>
+      <c r="O11" s="46"/>
     </row>
     <row r="12" spans="1:15" ht="150.75" thickBot="1">
       <c r="A12" s="17">
@@ -2958,29 +2956,27 @@
         <v>36</v>
       </c>
       <c r="F12" s="20">
-        <v>44974</v>
+        <v>45000</v>
       </c>
       <c r="G12" s="45" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="M12" s="22"/>
+        <v>91</v>
+      </c>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22" t="s">
+        <v>96</v>
+      </c>
       <c r="N12" s="23"/>
-      <c r="O12" s="58" t="s">
-        <v>108</v>
-      </c>
+      <c r="O12" s="46"/>
     </row>
     <row r="13" spans="1:15" ht="150.75" thickBot="1">
       <c r="A13" s="17">
@@ -2999,29 +2995,27 @@
         <v>38</v>
       </c>
       <c r="F13" s="20">
-        <v>44974</v>
+        <v>45000</v>
       </c>
       <c r="G13" s="45" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="H13" s="44" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="M13" s="22"/>
+        <v>91</v>
+      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22" t="s">
+        <v>96</v>
+      </c>
       <c r="N13" s="23"/>
-      <c r="O13" s="58" t="s">
-        <v>108</v>
-      </c>
+      <c r="O13" s="46"/>
     </row>
     <row r="14" spans="1:15" ht="120.75" thickBot="1">
       <c r="A14" s="17">
@@ -3043,16 +3037,16 @@
         <v>44974</v>
       </c>
       <c r="G14" s="45" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="H14" s="44" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="I14" s="44" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="J14" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>43</v>
@@ -3086,16 +3080,16 @@
         <v>44974</v>
       </c>
       <c r="G15" s="45" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="H15" s="44" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="I15" s="44" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="J15" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>43</v>
@@ -3130,7 +3124,7 @@
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
       <c r="J16" s="22" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>43</v>
@@ -3164,16 +3158,16 @@
         <v>44977</v>
       </c>
       <c r="G17" s="45" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="J17" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K17" s="22" t="s">
         <v>43</v>
@@ -3185,7 +3179,7 @@
       <c r="N17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="O17" s="58"/>
+      <c r="O17" s="46"/>
     </row>
     <row r="18" spans="1:15" ht="120.75" thickBot="1">
       <c r="A18" s="17">
@@ -3207,16 +3201,16 @@
         <v>44974</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="I18" s="44" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="J18" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K18" s="22" t="s">
         <v>43</v>
@@ -3250,16 +3244,16 @@
         <v>44974</v>
       </c>
       <c r="G19" s="45" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="I19" s="44" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="J19" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K19" s="22" t="s">
         <v>43</v>
@@ -3283,7 +3277,7 @@
       <c r="C20" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="48" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="19" t="s">
@@ -3293,16 +3287,16 @@
         <v>44977</v>
       </c>
       <c r="G20" s="44" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="H20" s="44" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="I20" s="44" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K20" s="43" t="s">
         <v>43</v>
@@ -3336,16 +3330,16 @@
         <v>44977</v>
       </c>
       <c r="G21" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" s="43" t="s">
         <v>127</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="J21" s="43" t="s">
-        <v>139</v>
       </c>
       <c r="K21" s="22" t="s">
         <v>43</v>
@@ -3379,16 +3373,16 @@
         <v>44977</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="J22" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K22" s="22" t="s">
         <v>43</v>
@@ -3422,16 +3416,16 @@
         <v>44977</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="J23" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K23" s="22" t="s">
         <v>43</v>
@@ -3465,16 +3459,16 @@
         <v>44977</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="J24" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K24" s="22" t="s">
         <v>43</v>
@@ -3574,16 +3568,16 @@
         <v>44977</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J27" s="43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K27" s="22" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Fix test non applicabili
Fix test non applicabili
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/emanuele_bianchi_dedalus_eu/Documents/Documenti/Production/FSE2.0/S1#111DEDALUS0000_SecondPR/DEDALUS/WHOSPITAL/28.6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/emanuele_bianchi_dedalus_eu/Documents/Documenti/Production/FSE2.0/S1#111DEDALUS0000_ThirdPR/DEDALUS/WHOSPITAL/28.6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="11_E5844F8BE441DE9AE0E2741B1C08B253CC0EFC9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EAA9EF-D5BB-4E9B-8E8E-DCF654B451EE}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="11_E5844F8BE441DE9AE0E2741B1C08B253CC0EFC9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C4F699B-AFE8-4966-B07A-FA8DF4957349}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="134">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -674,33 +674,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.30922.4.4.57eb4e049b0d33aeb034be70b5e9175d73e1e6d8b94dd9ef64cc27e90b4f5901.a01731730d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-15T10:23:25Z</t>
-  </si>
-  <si>
-    <t>c3cafdab2dda3a5e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.548fb5c0eea3e1f235feda2bf0962e5d9eb83833ec1d85e8b361515ebdd30c65.d46a21d443^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-15T10:31:03Z</t>
-  </si>
-  <si>
-    <t>dd15863c397c18d7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.cb3d023c0bca1ccc0ef42aa132e292243dac5f08f847ac9da0ea1316ad119b82.b621c5e9ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-15T10:36:49Z</t>
-  </si>
-  <si>
-    <t>b0825debc2f2aa97</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.8e09bb6d0d285f084c7e1e68c7806cc39296063545601bf6387cf5c84504c8aa.521e3ef2fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2664,10 +2637,10 @@
   <dimension ref="A1:O873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2916,18 +2889,10 @@
       <c r="E11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="20">
-        <v>45000</v>
-      </c>
-      <c r="G11" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>136</v>
-      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
         <v>91</v>
@@ -2955,18 +2920,10 @@
       <c r="E12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="20">
-        <v>45000</v>
-      </c>
-      <c r="G12" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>139</v>
-      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
         <v>91</v>
@@ -2994,18 +2951,10 @@
       <c r="E13" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="20">
-        <v>45000</v>
-      </c>
-      <c r="G13" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="H13" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I13" s="44" t="s">
-        <v>142</v>
-      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
RSA Fix report-checklist 29 e 37
RSA Fix report-checklist 29 e 37
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27424"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa.sharepoint.com/sites/wHospitalDev/Shared Documents/General/FSE-2.0/Validazione_LDO_RSA/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="571" documentId="11_D02697B058064E8558B1D8CE05CFACF2181887E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38AB398A-1B19-4157-B265-5CF184490F1D}"/>
+  <xr:revisionPtr revIDLastSave="573" documentId="11_D02697B058064E8558B1D8CE05CFACF2181887E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF1F6EC0-7955-41EE-A1DE-09EC1AE21610}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="340">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1833,7 +1833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1938,6 +1938,9 @@
     <xf numFmtId="14" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1952,15 +1955,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -4433,8 +4427,8 @@
   <dimension ref="A1:T673"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -4478,12 +4472,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="44"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4501,14 +4495,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="44"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4526,12 +4520,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="42" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4550,12 +4544,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="50"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="42" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4573,8 +4567,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4892,7 +4886,9 @@
       <c r="L14" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="M14" s="25"/>
+      <c r="M14" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="N14" s="25" t="s">
         <v>71</v>
       </c>
@@ -4910,7 +4906,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="198">
-      <c r="A15" s="45">
+      <c r="A15" s="38">
         <v>37</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -4944,7 +4940,9 @@
       <c r="L15" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="25"/>
+      <c r="M15" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="N15" s="25" t="s">
         <v>71</v>
       </c>
@@ -5006,7 +5004,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" ht="321">
-      <c r="A17" s="43">
+      <c r="A17" s="20">
         <v>63</v>
       </c>
       <c r="B17" s="21" t="s">
@@ -5276,7 +5274,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="321">
-      <c r="A22" s="43">
+      <c r="A22" s="20">
         <v>68</v>
       </c>
       <c r="B22" s="21" t="s">
@@ -5330,7 +5328,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" ht="409.6">
-      <c r="A23" s="43">
+      <c r="A23" s="20">
         <v>69</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -5384,7 +5382,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="305.25">
-      <c r="A24" s="43">
+      <c r="A24" s="20">
         <v>70</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -5514,7 +5512,7 @@
       </c>
     </row>
     <row r="27" spans="1:20" ht="321">
-      <c r="A27" s="43">
+      <c r="A27" s="20">
         <v>73</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -5554,7 +5552,7 @@
       <c r="N27" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="44" t="s">
+      <c r="O27" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P27" s="34" t="s">
@@ -14307,6 +14305,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851878ea-deef-4a3d-b773-69b426619c9b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MigrationWizIdPermissionLevels xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <MigrationWizIdDocumentLibraryPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <MigrationWizIdSecurityGroups xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <Status xmlns="851878ea-deef-4a3d-b773-69b426619c9b">Draft</Status>
+    <TaxCatchAll xmlns="76ffd0b7-0dc2-4bf2-8bb7-e61bc4d60314" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <MigrationWizId xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003D2D6B8F16614B49A029AB2437711D26" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8ae7918fb74eb172b1cee7479da6f18b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851878ea-deef-4a3d-b773-69b426619c9b" xmlns:ns3="76ffd0b7-0dc2-4bf2-8bb7-e61bc4d60314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="052140706cef89cf7bb41a9abdf09606" ns2:_="" ns3:_="">
     <xsd:import namespace="851878ea-deef-4a3d-b773-69b426619c9b"/>
@@ -14554,35 +14579,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851878ea-deef-4a3d-b773-69b426619c9b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MigrationWizIdPermissionLevels xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <MigrationWizIdDocumentLibraryPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <MigrationWizIdSecurityGroups xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <Status xmlns="851878ea-deef-4a3d-b773-69b426619c9b">Draft</Status>
-    <TaxCatchAll xmlns="76ffd0b7-0dc2-4bf2-8bb7-e61bc4d60314" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <MigrationWizId xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9077E48-1F09-404F-8E1A-1774FE5421F7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F98B64-4CA8-44E3-9A81-A1C71DB227F9}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14590,5 +14588,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F98B64-4CA8-44E3-9A81-A1C71DB227F9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9077E48-1F09-404F-8E1A-1774FE5421F7}"/>
 </file>
</xml_diff>

<commit_message>
Fix certificazione errori mail del 07/03
Fix certificazione errori mail del 07/03
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27504"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa.sharepoint.com/sites/wHospitalDev/Shared Documents/General/FSE-2.0/Validazione_LDO_RSA/S1#111DEDALUS0000/DEDALUS/WHOSPITAL/28.6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.genini\OneDrive - Dedalus S.p.A\Desktop\Validazione\Files per certificazione RSA_LDO\LDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="573" documentId="11_D02697B058064E8558B1D8CE05CFACF2181887E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF1F6EC0-7955-41EE-A1DE-09EC1AE21610}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{2C3EC839-737B-4C41-AFBE-6C2AFC3026F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FEC42A5-7AA8-45F3-9F97-823F04F4F352}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="338">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -324,19 +324,16 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-03-15T10:16:43Z</t>
-  </si>
-  <si>
-    <t>32024f65c5b09cd8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.57eb4e049b0d33aeb034be70b5e9175d73e1e6d8b94dd9ef64cc27e90b4f5901.a01731730d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T11:35:39Z</t>
+  </si>
+  <si>
+    <t>7a2aef4868cbd0ee</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.57eb4e049b0d33aeb034be70b5e9175d73e1e6d8b94dd9ef64cc27e90b4f5901.fbe68aa626^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>OK</t>
@@ -422,16 +419,16 @@
     </r>
   </si>
   <si>
-    <t>2023-02-17T17:01:17Z</t>
-  </si>
-  <si>
-    <t>46da14a311aa3db8</t>
+    <t>2024-03-12T09:54:42Z</t>
+  </si>
+  <si>
+    <t>6dc3bf080ed5eeef</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>Campo token JWT non valido</t>
+    <t>Campo token JWT non valido: Il campo subject_role non è valorizzato</t>
   </si>
   <si>
     <t>All'utente (medico) viene segnalato l'errore prima della validazione della LDO.
@@ -488,10 +485,13 @@
     </r>
   </si>
   <si>
-    <t>2023-02-17T17:08:46Z</t>
-  </si>
-  <si>
-    <t>84e76dcf1453bd26</t>
+    <t>2024-03-12T10:02:43Z</t>
+  </si>
+  <si>
+    <t>d97c54fdb9bbc104</t>
+  </si>
+  <si>
+    <t>Campo token JWT non valido: Il codice fiscale nel campo person_id non è corretto</t>
   </si>
   <si>
     <t>All'utente (medico) viene segnalato l'errore prima della validazione della LDO.
@@ -525,16 +525,16 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-20T15:36:10Z</t>
-  </si>
-  <si>
-    <t>1f4366324aa109ea</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.7357ebe77d8b19fad8fcfb510ed29df4b89c94412e7e5d6ac5f660e59b2d2407.6064d3e95e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Campo token JWT non valido. - non è stato possibile verificare il codice fiscale del paziente presente nel CDA</t>
+    <t>2024-03-11T16:00:04Z</t>
+  </si>
+  <si>
+    <t>f0739e20d9a68112</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.7c287cb475a284fde22810f96064dbad7deba1c6b7365a4b533fb84289e39faf.fb9d1b3213^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
   </si>
   <si>
     <t>Viene segnalato al medico, prima della validazione della LDO, il dettaglio dell'errore ricevuto dal gataway, es: 
@@ -553,20 +553,19 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-17T17:16:49Z</t>
-  </si>
-  <si>
-    <t>aa10cc785a931fab</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.80656725cce9221b755d34e497b89ecc65a4132e2b6bc193fe823ab7d23ffc28.654331430a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[Errore-47| codice fiscale 'fsettn99b09f205' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
-  </si>
-  <si>
-    <t>Viene segnalato al medico, prima della validazione della LDO, il dettaglio dell'errore ricevuto dal gataway, es: 
-"[Errore-47| codice fiscale 'fsettn99b09f205' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]"
+    <t>2024-03-11T11:39:42Z</t>
+  </si>
+  <si>
+    <t>e2d7d84b70b0ee8d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.80656725cce9221b755d34e497b89ecc65a4132e2b6bc193fe823ab7d23ffc28.87760ca832^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
+  </si>
+  <si>
+    <t>Viene segnalato al medico, prima della validazione della LDO, il dettaglio dell'errore ricevuto dal gataway, 
 Il medico può comunque proseguire e produrre il documento.
 La gestione dell'errore è in carico ad un operatore di back office.
 Una volta risolto il problema in back office ed effettuata la validazione il documento è automaticamente pubblicato</t>
@@ -580,13 +579,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-17T17:23:32Z</t>
-  </si>
-  <si>
-    <t>7d7ada9571ab8dd8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.52f1f2fa78c6594333731b1bd8a08641c34b2fdd69bf460c54687648f0a77781.5b8d8b4d2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T10:21:58Z</t>
+  </si>
+  <si>
+    <t>865b4c35448740a8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.52f1f2fa78c6594333731b1bd8a08641c34b2fdd69bf460c54687648f0a77781.919204574d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>[ERRORE-6| L'elemento 'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']</t>
@@ -608,13 +607,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-20T14:34:04Z</t>
-  </si>
-  <si>
-    <t>959246a4b973648f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.446ed6ffa3664a625b7f81c9e1f2c0494b90e8ab454355e71f274801ebef3025.718010990e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T10:29:11Z</t>
+  </si>
+  <si>
+    <t>649202c21276a48d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.446ed6ffa3664a625b7f81c9e1f2c0494b90e8ab454355e71f274801ebef3025.e7b4aac925^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve"> [ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
@@ -636,13 +635,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-20T13:59:39Z</t>
-  </si>
-  <si>
-    <t>20052051f97f317d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.bc398ec02d42511f3800879627404ecda2f7d3fdee9503ee5d0bd21c34044d33.597bb5c5ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T10:38:50Z</t>
+  </si>
+  <si>
+    <t>05b3a98244e5ff45</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.bc398ec02d42511f3800879627404ecda2f7d3fdee9503ee5d0bd21c34044d33.133582d242^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
@@ -664,13 +663,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-20T13:30:23Z</t>
-  </si>
-  <si>
-    <t>9aa41d3b3d558781</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.07f2d433f082c18c09b61c4d816802c4453e65c1afe8027bc3295f14214f2d2a.df995661fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T11:09:56Z</t>
+  </si>
+  <si>
+    <t>0adac0d3da883ed3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.07f2d433f082c18c09b61c4d816802c4453e65c1afe8027bc3295f14214f2d2a.48046bac27^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore vocabolario. ,detail= Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: O]</t>
@@ -692,13 +691,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-20T14:08:21Z</t>
-  </si>
-  <si>
-    <t>eec9c64918d70758</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.9d3cf05b2f6f5a366c52bc43fdf53bb647982debb59e8c2ef80b4e84d3c2df11.0da17e2981^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T11:15:30Z</t>
+  </si>
+  <si>
+    <t>929a1db380c35401</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.9d3cf05b2f6f5a366c52bc43fdf53bb647982debb59e8c2ef80b4e84d3c2df11.a2e7487d90^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
@@ -720,13 +719,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-20T14:16:37Z</t>
-  </si>
-  <si>
-    <t>6ac82a4ee56056a8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.85c2bc8e40185c09f8657c78831813bb145edd50b6a588ddd63c1832db78d10d.f6a3d38e16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T11:20:40Z</t>
+  </si>
+  <si>
+    <t>01b15b2ab35f17ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.85c2bc8e40185c09f8657c78831813bb145edd50b6a588ddd63c1832db78d10d.c349fec195^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve"> [ERRORE-b4| Sezione Decorso Ospedaliero: La sezione deve contenere l'elemento 'text']</t>
@@ -772,13 +771,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-02-20T13:48:31Z</t>
-  </si>
-  <si>
-    <t>448f51a789dc26bd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30922.4.4.60297f2bba79ec6f3fb7ea99906c1b00fa5f885fa7d840b062cf8d8fb861fd47.39134b0a4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-11T11:25:47Z</t>
+  </si>
+  <si>
+    <t>9bde49e1f9c35b7a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30922.4.4.60297f2bba79ec6f3fb7ea99906c1b00fa5f885fa7d840b062cf8d8fb861fd47.ab239626c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -878,9 +877,6 @@
     <t>271ccf1f763c0958</t>
   </si>
   <si>
-    <t>Campo token JWT non valido: Il campo subject_role non è valorizzato</t>
-  </si>
-  <si>
     <t>All'utente (medico) viene segnalato l'errore prima della validazione della RSA.
 Il medico può annullare l'operazione e tentare di risolvere il problema o proseguire comunque e produrre il documento.
 Prima della pubblicazione il sistema ritenta automaticamente la validazione.
@@ -938,9 +934,6 @@
     <t>d257504aed4502ca</t>
   </si>
   <si>
-    <t>Campo token JWT non valido: Il codice fiscale nel campo person_id non è corretto</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_RSA_TIMEOUT</t>
   </si>
   <si>
@@ -1030,9 +1023,6 @@
     <t>2.16.840.1.113883.2.9.2.30922.4.4.6670fcf1b903917a6de02488be32110b06d8cd8b9731c910f589e31efa3acb3f.16d8c0e222^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT7_KO</t>
   </si>
   <si>
@@ -1490,6 +1480,9 @@
   </si>
   <si>
     <t>Oscuramento</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -4426,9 +4419,9 @@
   </sheetPr>
   <dimension ref="A1:T673"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -4438,8 +4431,8 @@
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
-    <col min="5" max="5" width="104.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="5" max="5" width="69.42578125" customWidth="1"/>
     <col min="6" max="7" width="33.140625" customWidth="1"/>
     <col min="8" max="8" width="31.5703125" customWidth="1"/>
     <col min="9" max="9" width="33.140625" customWidth="1"/>
@@ -4685,7 +4678,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="39.75" customHeight="1" thickBot="1">
+    <row r="10" spans="1:20" ht="71.25" customHeight="1" thickBot="1">
       <c r="A10" s="20">
         <v>6</v>
       </c>
@@ -4702,7 +4695,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="23">
-        <v>45000</v>
+        <v>45362</v>
       </c>
       <c r="G10" s="36" t="s">
         <v>51</v>
@@ -4722,16 +4715,14 @@
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
-      <c r="Q10" s="34" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q10" s="34"/>
       <c r="R10" s="26"/>
       <c r="S10" s="27"/>
       <c r="T10" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="305.25" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="52.5" customHeight="1" thickBot="1">
       <c r="A11" s="20">
         <v>7</v>
       </c>
@@ -4742,36 +4733,36 @@
         <v>48</v>
       </c>
       <c r="D11" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>59</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>60</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="26"/>
       <c r="S11" s="27"/>
       <c r="T11" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="152.25" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="54" customHeight="1" thickBot="1">
       <c r="A12" s="20">
         <v>8</v>
       </c>
@@ -4782,36 +4773,36 @@
         <v>48</v>
       </c>
       <c r="D12" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>61</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>62</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
       <c r="J12" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
       <c r="P12" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="26"/>
       <c r="S12" s="27"/>
       <c r="T12" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="152.25" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="69" customHeight="1" thickBot="1">
       <c r="A13" s="20">
         <v>9</v>
       </c>
@@ -4822,36 +4813,36 @@
         <v>48</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>64</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
       <c r="J13" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q13" s="25"/>
       <c r="R13" s="26"/>
       <c r="S13" s="27"/>
       <c r="T13" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="229.5" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="77.25" customHeight="1" thickBot="1">
       <c r="A14" s="20">
         <v>29</v>
       </c>
@@ -4862,50 +4853,50 @@
         <v>48</v>
       </c>
       <c r="D14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="F14" s="23">
+        <v>45363</v>
+      </c>
+      <c r="G14" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="23">
-        <v>44974</v>
-      </c>
-      <c r="G14" s="36" t="s">
+      <c r="H14" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="I14" s="37" t="s">
         <v>69</v>
-      </c>
-      <c r="I14" s="37" t="s">
-        <v>70</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M14" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N14" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O14" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P14" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="26"/>
       <c r="S14" s="27"/>
       <c r="T14" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="198">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="82.5" customHeight="1" thickBot="1">
       <c r="A15" s="38">
         <v>37</v>
       </c>
@@ -4916,35 +4907,35 @@
         <v>48</v>
       </c>
       <c r="D15" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="F15" s="23">
+        <v>45363</v>
+      </c>
+      <c r="G15" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="23">
-        <v>44974</v>
-      </c>
-      <c r="G15" s="36" t="s">
+      <c r="H15" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="37" t="s">
-        <v>77</v>
-      </c>
       <c r="I15" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K15" s="25"/>
       <c r="L15" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M15" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>54</v>
@@ -4956,10 +4947,10 @@
       <c r="R15" s="26"/>
       <c r="S15" s="27"/>
       <c r="T15" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="198">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="120" customHeight="1" thickBot="1">
       <c r="A16" s="20">
         <v>45</v>
       </c>
@@ -4982,7 +4973,7 @@
       <c r="J16" s="25"/>
       <c r="K16" s="25"/>
       <c r="L16" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M16" s="25" t="s">
         <v>54</v>
@@ -5000,10 +4991,10 @@
       <c r="R16" s="26"/>
       <c r="S16" s="27"/>
       <c r="T16" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="321">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="71.25" customHeight="1" thickBot="1">
       <c r="A17" s="20">
         <v>63</v>
       </c>
@@ -5020,7 +5011,7 @@
         <v>84</v>
       </c>
       <c r="F17" s="23">
-        <v>44977</v>
+        <v>45362</v>
       </c>
       <c r="G17" s="36" t="s">
         <v>85</v>
@@ -5036,12 +5027,12 @@
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M17" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="N17" s="25" t="s">
+      <c r="N17" s="34" t="s">
         <v>88</v>
       </c>
       <c r="O17" s="25" t="s">
@@ -5054,10 +5045,10 @@
       <c r="R17" s="26"/>
       <c r="S17" s="27"/>
       <c r="T17" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="275.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="72.75" customHeight="1" thickBot="1">
       <c r="A18" s="20">
         <v>64</v>
       </c>
@@ -5074,7 +5065,7 @@
         <v>91</v>
       </c>
       <c r="F18" s="23">
-        <v>44974</v>
+        <v>45362</v>
       </c>
       <c r="G18" s="36" t="s">
         <v>92</v>
@@ -5090,7 +5081,7 @@
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M18" s="25" t="s">
         <v>54</v>
@@ -5108,10 +5099,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="27"/>
       <c r="T18" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="366">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="90" customHeight="1" thickBot="1">
       <c r="A19" s="20">
         <v>65</v>
       </c>
@@ -5128,7 +5119,7 @@
         <v>98</v>
       </c>
       <c r="F19" s="23">
-        <v>44974</v>
+        <v>45362</v>
       </c>
       <c r="G19" s="36" t="s">
         <v>99</v>
@@ -5144,7 +5135,7 @@
       </c>
       <c r="K19" s="25"/>
       <c r="L19" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M19" s="25" t="s">
         <v>54</v>
@@ -5162,10 +5153,10 @@
       <c r="R19" s="26"/>
       <c r="S19" s="27"/>
       <c r="T19" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="351">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="87" customHeight="1" thickBot="1">
       <c r="A20" s="20">
         <v>66</v>
       </c>
@@ -5182,7 +5173,7 @@
         <v>105</v>
       </c>
       <c r="F20" s="23">
-        <v>44977</v>
+        <v>45362</v>
       </c>
       <c r="G20" s="37" t="s">
         <v>106</v>
@@ -5198,7 +5189,7 @@
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M20" s="25" t="s">
         <v>54</v>
@@ -5216,10 +5207,10 @@
       <c r="R20" s="26"/>
       <c r="S20" s="27"/>
       <c r="T20" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="336">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="90.75" customHeight="1" thickBot="1">
       <c r="A21" s="20">
         <v>67</v>
       </c>
@@ -5236,7 +5227,7 @@
         <v>112</v>
       </c>
       <c r="F21" s="23">
-        <v>44977</v>
+        <v>45362</v>
       </c>
       <c r="G21" s="37" t="s">
         <v>113</v>
@@ -5252,7 +5243,7 @@
       </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M21" s="25" t="s">
         <v>54</v>
@@ -5270,10 +5261,10 @@
       <c r="R21" s="26"/>
       <c r="S21" s="27"/>
       <c r="T21" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="321">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="113.25" customHeight="1" thickBot="1">
       <c r="A22" s="20">
         <v>68</v>
       </c>
@@ -5290,7 +5281,7 @@
         <v>119</v>
       </c>
       <c r="F22" s="23">
-        <v>44977</v>
+        <v>45362</v>
       </c>
       <c r="G22" s="37" t="s">
         <v>120</v>
@@ -5306,7 +5297,7 @@
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M22" s="25" t="s">
         <v>54</v>
@@ -5324,10 +5315,10 @@
       <c r="R22" s="26"/>
       <c r="S22" s="27"/>
       <c r="T22" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="409.6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="93" customHeight="1" thickBot="1">
       <c r="A23" s="20">
         <v>69</v>
       </c>
@@ -5344,7 +5335,7 @@
         <v>126</v>
       </c>
       <c r="F23" s="23">
-        <v>44977</v>
+        <v>45362</v>
       </c>
       <c r="G23" s="37" t="s">
         <v>127</v>
@@ -5360,7 +5351,7 @@
       </c>
       <c r="K23" s="25"/>
       <c r="L23" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M23" s="25" t="s">
         <v>54</v>
@@ -5378,10 +5369,10 @@
       <c r="R23" s="26"/>
       <c r="S23" s="27"/>
       <c r="T23" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="305.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="101.25" customHeight="1" thickBot="1">
       <c r="A24" s="20">
         <v>70</v>
       </c>
@@ -5398,7 +5389,7 @@
         <v>133</v>
       </c>
       <c r="F24" s="23">
-        <v>44977</v>
+        <v>45362</v>
       </c>
       <c r="G24" s="37" t="s">
         <v>134</v>
@@ -5414,7 +5405,7 @@
       </c>
       <c r="K24" s="25"/>
       <c r="L24" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M24" s="25" t="s">
         <v>54</v>
@@ -5432,10 +5423,10 @@
       <c r="R24" s="26"/>
       <c r="S24" s="27"/>
       <c r="T24" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="121.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="120">
       <c r="A25" s="20">
         <v>71</v>
       </c>
@@ -5456,7 +5447,7 @@
       <c r="H25" s="37"/>
       <c r="I25" s="37"/>
       <c r="J25" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K25" s="34" t="s">
         <v>141</v>
@@ -5470,10 +5461,10 @@
       <c r="R25" s="26"/>
       <c r="S25" s="27"/>
       <c r="T25" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="121.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="120.75" thickBot="1">
       <c r="A26" s="20">
         <v>72</v>
       </c>
@@ -5494,7 +5485,7 @@
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
       <c r="J26" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K26" s="34" t="s">
         <v>144</v>
@@ -5508,10 +5499,10 @@
       <c r="R26" s="26"/>
       <c r="S26" s="27"/>
       <c r="T26" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="321">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="90.75" customHeight="1" thickBot="1">
       <c r="A27" s="20">
         <v>73</v>
       </c>
@@ -5528,7 +5519,7 @@
         <v>146</v>
       </c>
       <c r="F27" s="23">
-        <v>44977</v>
+        <v>45362</v>
       </c>
       <c r="G27" s="37" t="s">
         <v>147</v>
@@ -5544,7 +5535,7 @@
       </c>
       <c r="K27" s="34"/>
       <c r="L27" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M27" s="25" t="s">
         <v>150</v>
@@ -5562,10 +5553,10 @@
       <c r="R27" s="26"/>
       <c r="S27" s="27"/>
       <c r="T27" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="50.25" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="144" customHeight="1" thickBot="1">
       <c r="A28" s="20">
         <v>74</v>
       </c>
@@ -5586,7 +5577,7 @@
       <c r="H28" s="24"/>
       <c r="I28" s="24"/>
       <c r="J28" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K28" s="34" t="s">
         <v>155</v>
@@ -5600,10 +5591,10 @@
       <c r="R28" s="26"/>
       <c r="S28" s="27"/>
       <c r="T28" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="152.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="150">
       <c r="A29" s="20">
         <v>369</v>
       </c>
@@ -5644,7 +5635,7 @@
       <c r="R29" s="26"/>
       <c r="S29" s="27"/>
       <c r="T29" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="188.25" customHeight="1">
@@ -5673,32 +5664,32 @@
         <v>165</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J30" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K30" s="25"/>
       <c r="L30" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M30" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N30" s="25" t="s">
-        <v>166</v>
+        <v>70</v>
       </c>
       <c r="O30" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P30" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="26"/>
       <c r="S30" s="27"/>
       <c r="T30" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="167.25" customHeight="1">
@@ -5712,50 +5703,50 @@
         <v>161</v>
       </c>
       <c r="D31" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" s="33" t="s">
         <v>168</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>169</v>
       </c>
       <c r="F31" s="23">
         <v>45343</v>
       </c>
       <c r="G31" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="H31" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="H31" s="24" t="s">
-        <v>171</v>
-      </c>
       <c r="I31" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J31" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K31" s="25"/>
       <c r="L31" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M31" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N31" s="25" t="s">
-        <v>172</v>
+        <v>77</v>
       </c>
       <c r="O31" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P31" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="26"/>
       <c r="S31" s="27"/>
       <c r="T31" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="198">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="210">
       <c r="A32" s="20">
         <v>48</v>
       </c>
@@ -5766,7 +5757,7 @@
         <v>161</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E32" s="22" t="s">
         <v>80</v>
@@ -5778,7 +5769,7 @@
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
       <c r="L32" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M32" s="25" t="s">
         <v>54</v>
@@ -5796,7 +5787,7 @@
       <c r="R32" s="26"/>
       <c r="S32" s="27"/>
       <c r="T32" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="138" customHeight="1" thickBot="1">
@@ -5810,20 +5801,20 @@
         <v>161</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
       <c r="J33" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K33" s="25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
@@ -5834,10 +5825,10 @@
       <c r="R33" s="26"/>
       <c r="S33" s="27"/>
       <c r="T33" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="167.25" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="165.75" thickBot="1">
       <c r="A34" s="20">
         <v>148</v>
       </c>
@@ -5848,20 +5839,20 @@
         <v>161</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F34" s="23"/>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
       <c r="I34" s="24"/>
       <c r="J34" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K34" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
@@ -5872,10 +5863,10 @@
       <c r="R34" s="26"/>
       <c r="S34" s="27"/>
       <c r="T34" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="167.25" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="165.75" thickBot="1">
       <c r="A35" s="20">
         <v>149</v>
       </c>
@@ -5886,20 +5877,20 @@
         <v>161</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
       <c r="J35" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
@@ -5910,10 +5901,10 @@
       <c r="R35" s="26"/>
       <c r="S35" s="27"/>
       <c r="T35" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="167.25" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="165.75" thickBot="1">
       <c r="A36" s="20">
         <v>150</v>
       </c>
@@ -5924,20 +5915,20 @@
         <v>161</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
       <c r="J36" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -5948,7 +5939,7 @@
       <c r="R36" s="26"/>
       <c r="S36" s="27"/>
       <c r="T36" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="177.75" customHeight="1" thickBot="1">
@@ -5962,47 +5953,47 @@
         <v>161</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F37" s="23">
         <v>45335</v>
       </c>
       <c r="G37" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="I37" s="24" t="s">
         <v>188</v>
-      </c>
-      <c r="H37" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="I37" s="24" t="s">
-        <v>190</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K37" s="25"/>
       <c r="L37" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M37" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N37" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="O37" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P37" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
       <c r="S37" s="27"/>
       <c r="T37" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="174.75" customHeight="1" thickBot="1">
@@ -6016,47 +6007,47 @@
         <v>161</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F38" s="23">
         <v>45335</v>
       </c>
       <c r="G38" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="I38" s="24" t="s">
         <v>194</v>
-      </c>
-      <c r="H38" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="I38" s="24" t="s">
-        <v>196</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K38" s="25"/>
       <c r="L38" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M38" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N38" s="25" t="s">
-        <v>197</v>
+        <v>95</v>
       </c>
       <c r="O38" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P38" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="26"/>
       <c r="S38" s="27"/>
       <c r="T38" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="138.75" customHeight="1" thickBot="1">
@@ -6070,47 +6061,47 @@
         <v>161</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F39" s="23">
         <v>45335</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K39" s="25"/>
       <c r="L39" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M39" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N39" s="25" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="O39" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P39" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
       <c r="S39" s="27"/>
       <c r="T39" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="155.25" customHeight="1" thickBot="1">
@@ -6124,47 +6115,47 @@
         <v>161</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F40" s="23">
         <v>45335</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K40" s="25"/>
       <c r="L40" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M40" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="O40" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P40" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="26"/>
       <c r="S40" s="27"/>
       <c r="T40" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="127.5" customHeight="1" thickBot="1">
@@ -6178,29 +6169,29 @@
         <v>161</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F41" s="23">
         <v>45335</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H41" s="35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K41" s="25"/>
       <c r="L41" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M41" s="25" t="s">
         <v>54</v>
@@ -6212,13 +6203,13 @@
         <v>54</v>
       </c>
       <c r="P41" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="26"/>
       <c r="S41" s="27"/>
       <c r="T41" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="108" customHeight="1" thickBot="1">
@@ -6232,50 +6223,50 @@
         <v>161</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F42" s="23">
         <v>45335</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H42" s="35" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J42" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K42" s="25"/>
       <c r="L42" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M42" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N42" s="25" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O42" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P42" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q42" s="25"/>
       <c r="R42" s="26"/>
       <c r="S42" s="27"/>
       <c r="T42" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="121.5" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="135.75" thickBot="1">
       <c r="A43" s="20">
         <v>157</v>
       </c>
@@ -6286,20 +6277,20 @@
         <v>161</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F43" s="23"/>
       <c r="G43" s="24"/>
       <c r="H43" s="24"/>
       <c r="I43" s="24"/>
       <c r="J43" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K43" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L43" s="25"/>
       <c r="M43" s="25"/>
@@ -6310,10 +6301,10 @@
       <c r="R43" s="26"/>
       <c r="S43" s="27"/>
       <c r="T43" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="121.5" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="135.75" thickBot="1">
       <c r="A44" s="20">
         <v>158</v>
       </c>
@@ -6324,20 +6315,20 @@
         <v>161</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F44" s="23"/>
       <c r="G44" s="24"/>
       <c r="H44" s="24"/>
       <c r="I44" s="24"/>
       <c r="J44" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K44" s="25" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L44" s="25"/>
       <c r="M44" s="25"/>
@@ -6348,10 +6339,10 @@
       <c r="R44" s="26"/>
       <c r="S44" s="27"/>
       <c r="T44" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="229.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="240">
       <c r="A45" s="20">
         <v>159</v>
       </c>
@@ -6362,50 +6353,50 @@
         <v>161</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F45" s="23">
         <v>45338</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K45" s="25"/>
       <c r="L45" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M45" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N45" s="25" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P45" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
       <c r="S45" s="27"/>
       <c r="T45" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="229.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="240">
       <c r="A46" s="20">
         <v>160</v>
       </c>
@@ -6416,52 +6407,52 @@
         <v>161</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F46" s="23">
         <v>45337</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K46" s="25"/>
       <c r="L46" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M46" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N46" s="25" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P46" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
       <c r="S46" s="34" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="T46" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="229.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="240">
       <c r="A47" s="20">
         <v>161</v>
       </c>
@@ -6472,50 +6463,50 @@
         <v>161</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F47" s="23">
         <v>45336</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H47" s="35" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K47" s="25"/>
       <c r="L47" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M47" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P47" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
       <c r="S47" s="27"/>
       <c r="T47" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="229.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="240">
       <c r="A48" s="20">
         <v>162</v>
       </c>
@@ -6526,50 +6517,50 @@
         <v>161</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F48" s="23">
         <v>45336</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H48" s="35" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="J48" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K48" s="25"/>
       <c r="L48" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M48" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P48" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="26"/>
       <c r="S48" s="27"/>
       <c r="T48" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" ht="229.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="240">
       <c r="A49" s="20">
         <v>163</v>
       </c>
@@ -6580,50 +6571,50 @@
         <v>161</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F49" s="23">
         <v>45336</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H49" s="35" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I49" s="24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J49" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K49" s="25"/>
       <c r="L49" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M49" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N49" s="25" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O49" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P49" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q49" s="25"/>
       <c r="R49" s="26"/>
       <c r="S49" s="27"/>
       <c r="T49" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" ht="121.5" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="135.75" thickBot="1">
       <c r="A50" s="20">
         <v>164</v>
       </c>
@@ -6634,20 +6625,20 @@
         <v>161</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F50" s="23"/>
       <c r="G50" s="24"/>
       <c r="H50" s="24"/>
       <c r="I50" s="24"/>
       <c r="J50" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K50" s="25" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="L50" s="25"/>
       <c r="M50" s="25"/>
@@ -6658,10 +6649,10 @@
       <c r="R50" s="26"/>
       <c r="S50" s="27"/>
       <c r="T50" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" ht="121.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="135">
       <c r="A51" s="20">
         <v>165</v>
       </c>
@@ -6672,20 +6663,20 @@
         <v>161</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F51" s="23"/>
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
       <c r="I51" s="24"/>
       <c r="J51" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K51" s="25" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="L51" s="25"/>
       <c r="M51" s="25"/>
@@ -6696,7 +6687,7 @@
       <c r="R51" s="26"/>
       <c r="S51" s="27"/>
       <c r="T51" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="237" customHeight="1" thickBot="1">
@@ -6710,20 +6701,20 @@
         <v>161</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F52" s="23"/>
       <c r="G52" s="24"/>
       <c r="H52" s="24"/>
       <c r="I52" s="24"/>
       <c r="J52" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K52" s="25" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L52" s="25"/>
       <c r="M52" s="25"/>
@@ -6734,10 +6725,10 @@
       <c r="R52" s="26"/>
       <c r="S52" s="27"/>
       <c r="T52" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" ht="121.5" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="135.75" thickBot="1">
       <c r="A53" s="20">
         <v>167</v>
       </c>
@@ -6748,20 +6739,20 @@
         <v>161</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F53" s="23"/>
       <c r="G53" s="24"/>
       <c r="H53" s="24"/>
       <c r="I53" s="24"/>
       <c r="J53" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K53" s="25" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L53" s="25"/>
       <c r="M53" s="25"/>
@@ -6772,10 +6763,10 @@
       <c r="R53" s="26"/>
       <c r="S53" s="27"/>
       <c r="T53" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" ht="121.5" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="135.75" thickBot="1">
       <c r="A54" s="20">
         <v>168</v>
       </c>
@@ -6786,20 +6777,20 @@
         <v>161</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="24"/>
       <c r="H54" s="24"/>
       <c r="I54" s="24"/>
       <c r="J54" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K54" s="25" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="L54" s="25"/>
       <c r="M54" s="25"/>
@@ -6810,10 +6801,10 @@
       <c r="R54" s="26"/>
       <c r="S54" s="27"/>
       <c r="T54" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" ht="229.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" ht="240">
       <c r="A55" s="20">
         <v>169</v>
       </c>
@@ -6824,47 +6815,47 @@
         <v>161</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F55" s="23">
         <v>45337</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J55" s="25" t="s">
         <v>54</v>
       </c>
       <c r="K55" s="25"/>
       <c r="L55" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M55" s="25" t="s">
         <v>54</v>
       </c>
       <c r="N55" s="25" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O55" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P55" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26"/>
       <c r="S55" s="27"/>
       <c r="T55" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="107.25" customHeight="1">
@@ -6878,22 +6869,22 @@
         <v>161</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F56" s="23">
         <v>45334</v>
       </c>
       <c r="G56" s="24" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I56" s="24" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J56" s="25" t="s">
         <v>54</v>
@@ -6908,7 +6899,7 @@
       <c r="R56" s="26"/>
       <c r="S56" s="27"/>
       <c r="T56" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="14.25" customHeight="1">
@@ -11609,24 +11600,24 @@
         <v>28</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
       <c r="A2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>284</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
@@ -11634,69 +11625,69 @@
         <v>48</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>285</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>288</v>
-      </c>
       <c r="D3" s="30" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11704,55 +11695,55 @@
         <v>161</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45">
       <c r="A10" s="11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C11" s="30">
         <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1">
@@ -11760,69 +11751,69 @@
         <v>48</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C12" s="30">
         <v>208</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C13" s="30">
         <v>224</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C14" s="30">
         <v>240</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C15" s="30">
         <v>256</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C16" s="30">
         <v>272</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
@@ -11830,41 +11821,41 @@
         <v>161</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C17" s="30">
         <v>288</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C18" s="30">
         <v>304</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C19" s="30">
         <v>193</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
@@ -11872,69 +11863,69 @@
         <v>48</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C20" s="30">
         <v>209</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C21" s="30">
         <v>225</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C22" s="30">
         <v>241</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C23" s="30">
         <v>257</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C24" s="30">
         <v>273</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
@@ -11942,41 +11933,41 @@
         <v>161</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C25" s="30">
         <v>289</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C26" s="30">
         <v>305</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C27" s="30">
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
@@ -11984,69 +11975,69 @@
         <v>48</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C28" s="30">
         <v>210</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C29" s="30">
         <v>226</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C30" s="30">
         <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C31" s="30">
         <v>258</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C32" s="30">
         <v>274</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
@@ -12054,35 +12045,35 @@
         <v>161</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C33" s="30">
         <v>290</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C34" s="30">
         <v>306</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C35" s="30">
         <v>195</v>
@@ -12096,7 +12087,7 @@
         <v>48</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C36" s="30">
         <v>211</v>
@@ -12107,10 +12098,10 @@
     </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C37" s="30">
         <v>227</v>
@@ -12121,10 +12112,10 @@
     </row>
     <row r="38" spans="1:4" ht="14.25" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C38" s="30">
         <v>243</v>
@@ -12135,10 +12126,10 @@
     </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1">
       <c r="A39" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C39" s="30">
         <v>259</v>
@@ -12149,10 +12140,10 @@
     </row>
     <row r="40" spans="1:4" ht="14.25" customHeight="1">
       <c r="A40" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C40" s="30">
         <v>275</v>
@@ -12166,7 +12157,7 @@
         <v>161</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C41" s="30">
         <v>291</v>
@@ -12177,10 +12168,10 @@
     </row>
     <row r="42" spans="1:4" ht="14.25" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C42" s="30">
         <v>307</v>
@@ -12191,10 +12182,10 @@
     </row>
     <row r="43" spans="1:4" ht="14.25" customHeight="1">
       <c r="A43" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C43" s="30">
         <v>196</v>
@@ -12208,7 +12199,7 @@
         <v>48</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C44" s="30">
         <v>212</v>
@@ -12219,10 +12210,10 @@
     </row>
     <row r="45" spans="1:4" ht="14.25" customHeight="1">
       <c r="A45" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C45" s="30">
         <v>228</v>
@@ -12233,10 +12224,10 @@
     </row>
     <row r="46" spans="1:4" ht="14.25" customHeight="1">
       <c r="A46" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C46" s="30">
         <v>244</v>
@@ -12247,10 +12238,10 @@
     </row>
     <row r="47" spans="1:4" ht="14.25" customHeight="1">
       <c r="A47" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C47" s="30">
         <v>260</v>
@@ -12261,10 +12252,10 @@
     </row>
     <row r="48" spans="1:4" ht="14.25" customHeight="1">
       <c r="A48" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C48" s="30">
         <v>276</v>
@@ -12278,7 +12269,7 @@
         <v>161</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C49" s="30">
         <v>292</v>
@@ -12289,10 +12280,10 @@
     </row>
     <row r="50" spans="1:4" ht="14.25" customHeight="1">
       <c r="A50" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C50" s="30">
         <v>308</v>
@@ -13280,7 +13271,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>336</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>54</v>
@@ -13288,10 +13279,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">
@@ -14305,24 +14296,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851878ea-deef-4a3d-b773-69b426619c9b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MigrationWizIdPermissionLevels xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <MigrationWizIdDocumentLibraryPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <MigrationWizIdSecurityGroups xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <Status xmlns="851878ea-deef-4a3d-b773-69b426619c9b">Draft</Status>
-    <TaxCatchAll xmlns="76ffd0b7-0dc2-4bf2-8bb7-e61bc4d60314" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-    <MigrationWizId xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -14331,7 +14304,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003D2D6B8F16614B49A029AB2437711D26" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8ae7918fb74eb172b1cee7479da6f18b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851878ea-deef-4a3d-b773-69b426619c9b" xmlns:ns3="76ffd0b7-0dc2-4bf2-8bb7-e61bc4d60314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="052140706cef89cf7bb41a9abdf09606" ns2:_="" ns3:_="">
     <xsd:import namespace="851878ea-deef-4a3d-b773-69b426619c9b"/>
@@ -14579,14 +14552,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851878ea-deef-4a3d-b773-69b426619c9b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MigrationWizIdPermissionLevels xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <MigrationWizIdDocumentLibraryPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <MigrationWizIdSecurityGroups xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <Status xmlns="851878ea-deef-4a3d-b773-69b426619c9b">Draft</Status>
+    <TaxCatchAll xmlns="76ffd0b7-0dc2-4bf2-8bb7-e61bc4d60314" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+    <MigrationWizId xmlns="851878ea-deef-4a3d-b773-69b426619c9b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F98B64-4CA8-44E3-9A81-A1C71DB227F9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A34496D-D45E-465E-BB75-C57361D9E54C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A34496D-D45E-465E-BB75-C57361D9E54C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{953B5FC0-8A3A-4ABA-A4FE-088B2494B76D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9077E48-1F09-404F-8E1A-1774FE5421F7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F98B64-4CA8-44E3-9A81-A1C71DB227F9}"/>
 </file>
</xml_diff>